<commit_message>
added ML churn project
</commit_message>
<xml_diff>
--- a/parsing the last one/Дневник_стажировки_Цифровое_лето.xlsx
+++ b/parsing the last one/Дневник_стажировки_Цифровое_лето.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Assiya.Karatay\Desktop\digital-summer-kcell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\8 semester\digital-summer-kcell\parsing the last one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2F5CBB-40DE-4C7B-986F-2A1F4EB2D562}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470"/>
   </bookViews>
   <sheets>
     <sheet name="Дневник стажировки" sheetId="1" r:id="rId1"/>
@@ -212,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -514,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -791,14 +790,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31998,7 +31997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>